<commit_message>
add 雷火之星, 埃迪卡拉级, CAS066(D), CV-M011(C), AT021
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\work\tc\lagrange\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A1BE1A-3400-4749-8941-BE6B2F95A955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D624BE21-126D-4E84-AA8E-A732F84A0EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12266" yWindow="1423" windowWidth="19594" windowHeight="15908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3394" yWindow="2606" windowWidth="21977" windowHeight="15908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="保底" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">保底!$A$1:$O$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">保底!$A$1:$O$115</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="171">
   <si>
     <t>SC002</t>
   </si>
@@ -654,6 +654,54 @@
   </si>
   <si>
     <t>2.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷火之星</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>埃迪卡拉级</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AT021</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>脉冲型(A)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">干扰型(B) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>多功能型(C)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>支援型(D)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>高速型(C)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1012,13 +1060,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O108"/>
+  <dimension ref="A1:O118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C81" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D105" sqref="D105"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -1139,22 +1187,22 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="D5" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" s="1">
         <v>1</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>1</v>
       </c>
       <c r="O5" s="1">
@@ -1166,16 +1214,19 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
         <v>1</v>
       </c>
       <c r="O6" s="1">
@@ -1187,19 +1238,16 @@
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="O7" s="1">
@@ -1208,19 +1256,22 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="D8" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <v>1</v>
       </c>
       <c r="O8" s="1">
@@ -1229,108 +1280,107 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>152</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-      <c r="L9" s="1">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>151</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="E10" s="1">
+        <v>162</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="L10" s="1">
-        <v>1</v>
-      </c>
-      <c r="O10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>151</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1">
+        <v>152</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5">
         <v>2.5</v>
       </c>
-      <c r="G12" s="1">
+      <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D13" s="5">
         <v>2.5</v>
       </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
         <v>1</v>
       </c>
       <c r="O13" s="1">
@@ -1342,13 +1392,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -1359,21 +1409,24 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
       </c>
       <c r="L15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1385,7 +1438,7 @@
         <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="5">
         <v>5</v>
@@ -1402,24 +1455,18 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D17" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1">
-        <v>1</v>
-      </c>
-      <c r="O17" s="1">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1428,24 +1475,18 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D18" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="O18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1457,7 +1498,7 @@
         <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="5">
         <v>2.5</v>
@@ -1465,6 +1506,9 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
       <c r="K19" s="1">
         <v>1</v>
       </c>
@@ -1474,13 +1518,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20" s="5">
         <v>2.5</v>
@@ -1488,7 +1532,13 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
-      <c r="N20" s="1">
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1497,10 +1547,10 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D21" s="5">
         <v>2.5</v>
@@ -1508,30 +1558,27 @@
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="L21" s="1">
-        <v>1</v>
-      </c>
-      <c r="N21" s="1">
+      <c r="K21" s="1">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="5">
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="J22" s="1">
         <v>1</v>
       </c>
       <c r="N22" s="1">
@@ -1543,18 +1590,18 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
         <v>1</v>
       </c>
       <c r="N23" s="1">
@@ -1566,15 +1613,15 @@
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="J24" s="1">
@@ -1592,12 +1639,15 @@
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" s="5">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
         <v>1</v>
       </c>
       <c r="N25" s="1">
@@ -1609,13 +1659,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D26" s="5">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1623,36 +1673,27 @@
       <c r="J26" s="1">
         <v>1</v>
       </c>
-      <c r="K26" s="1">
-        <v>1</v>
-      </c>
-      <c r="O26" s="1">
+      <c r="N26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="5">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1</v>
-      </c>
-      <c r="O27" s="1">
+      <c r="N27" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1664,7 +1705,7 @@
         <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="5">
         <v>2.5</v>
@@ -1684,18 +1725,18 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5">
-        <v>5</v>
-      </c>
-      <c r="H29" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E29" s="1">
         <v>1</v>
       </c>
       <c r="J29" s="1">
@@ -1704,7 +1745,7 @@
       <c r="K29" s="1">
         <v>1</v>
       </c>
-      <c r="N29" s="1">
+      <c r="O29" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1713,18 +1754,21 @@
         <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D30" s="5">
-        <v>5</v>
-      </c>
-      <c r="H30" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
         <v>1</v>
       </c>
       <c r="O30" s="1">
@@ -1739,24 +1783,33 @@
         <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="5">
         <v>5</v>
       </c>
       <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="N31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" s="5">
         <v>5</v>
@@ -1767,10 +1820,7 @@
       <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="L32" s="1">
-        <v>1</v>
-      </c>
-      <c r="N32" s="1">
+      <c r="O32" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1779,41 +1829,35 @@
         <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="5">
         <v>5</v>
       </c>
       <c r="H33" s="1">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1">
-        <v>1</v>
-      </c>
-      <c r="O33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="5">
-        <v>5</v>
+        <v>167</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
       </c>
-      <c r="O34" s="1">
+      <c r="L34" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1825,35 +1869,41 @@
         <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D35" s="5">
         <v>5</v>
       </c>
       <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="N35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D36" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F36" s="1">
+        <v>5</v>
+      </c>
+      <c r="H36" s="1">
         <v>1</v>
       </c>
       <c r="J36" s="1">
-        <v>1</v>
-      </c>
-      <c r="K36" s="1">
         <v>1</v>
       </c>
       <c r="O36" s="1">
@@ -1862,24 +1912,18 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D37" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="J37" s="1">
-        <v>1</v>
-      </c>
-      <c r="K37" s="1">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1">
         <v>1</v>
       </c>
       <c r="O37" s="1">
@@ -1888,24 +1932,18 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="D38" s="5">
         <v>5</v>
       </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1</v>
-      </c>
-      <c r="O38" s="1">
+      <c r="H38" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1914,21 +1952,24 @@
         <v>13</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D39" s="5">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="J39" s="1">
         <v>1</v>
       </c>
-      <c r="N39" s="1">
+      <c r="K39" s="1">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1937,18 +1978,24 @@
         <v>13</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D40" s="5">
         <v>2.5</v>
       </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="N40" s="1">
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
+      <c r="O40" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1957,21 +2004,21 @@
         <v>13</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="D41" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="G41" s="1">
-        <v>1</v>
-      </c>
-      <c r="L41" s="1">
-        <v>1</v>
-      </c>
-      <c r="N41" s="1">
+        <v>5</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+      <c r="O41" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1980,24 +2027,21 @@
         <v>13</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D42" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="G42" s="1">
+        <v>5</v>
+      </c>
+      <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="J42" s="1">
         <v>1</v>
       </c>
-      <c r="K42" s="1">
-        <v>1</v>
-      </c>
-      <c r="O42" s="1">
+      <c r="N42" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2006,18 +2050,15 @@
         <v>13</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="D43" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="J43" s="1">
         <v>1</v>
       </c>
       <c r="N43" s="1">
@@ -2029,18 +2070,18 @@
         <v>13</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D44" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
       </c>
-      <c r="J44" s="1">
+      <c r="L44" s="1">
         <v>1</v>
       </c>
       <c r="N44" s="1">
@@ -2052,64 +2093,70 @@
         <v>13</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G45" s="1">
         <v>1</v>
       </c>
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
       <c r="K45" s="1">
         <v>1</v>
       </c>
-      <c r="L45" s="1">
-        <v>1</v>
-      </c>
-      <c r="N45" s="1">
+      <c r="O45" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D46" s="5">
         <v>5</v>
       </c>
-      <c r="F46" s="1">
-        <v>1</v>
-      </c>
-      <c r="L46" s="1">
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D47" s="5">
         <v>5</v>
       </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="L47" s="1">
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2118,76 +2165,64 @@
         <v>13</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D48" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-      <c r="J48" s="1">
+        <v>5</v>
+      </c>
+      <c r="G48" s="1">
         <v>1</v>
       </c>
       <c r="K48" s="1">
         <v>1</v>
       </c>
-      <c r="O48" s="1">
+      <c r="L48" s="1">
+        <v>1</v>
+      </c>
+      <c r="N48" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D49" s="5">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
-      <c r="J49" s="1">
-        <v>1</v>
-      </c>
-      <c r="K49" s="1">
-        <v>1</v>
-      </c>
-      <c r="O49" s="1">
+      <c r="L49" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="D50" s="5">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
-      <c r="K50" s="1">
-        <v>1</v>
-      </c>
       <c r="L50" s="1">
-        <v>1</v>
-      </c>
-      <c r="O50" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2196,18 +2231,24 @@
         <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D51" s="5">
-        <v>5</v>
-      </c>
-      <c r="E51" s="1">
-        <v>1</v>
-      </c>
-      <c r="L51" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1">
+        <v>1</v>
+      </c>
+      <c r="O51" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2216,18 +2257,24 @@
         <v>13</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D52" s="5">
-        <v>5</v>
-      </c>
-      <c r="E52" s="1">
-        <v>1</v>
-      </c>
-      <c r="L52" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2236,18 +2283,24 @@
         <v>13</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="D53" s="5">
-        <v>5</v>
-      </c>
-      <c r="E53" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="K53" s="1">
         <v>1</v>
       </c>
       <c r="L53" s="1">
+        <v>1</v>
+      </c>
+      <c r="O53" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2256,10 +2309,10 @@
         <v>13</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D54" s="5">
         <v>5</v>
@@ -2268,9 +2321,6 @@
         <v>1</v>
       </c>
       <c r="L54" s="1">
-        <v>1</v>
-      </c>
-      <c r="O54" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2279,10 +2329,10 @@
         <v>13</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D55" s="5">
         <v>5</v>
@@ -2290,13 +2340,7 @@
       <c r="E55" s="1">
         <v>1</v>
       </c>
-      <c r="J55" s="1">
-        <v>1</v>
-      </c>
-      <c r="K55" s="1">
-        <v>1</v>
-      </c>
-      <c r="O55" s="1">
+      <c r="L55" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2305,10 +2349,10 @@
         <v>13</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D56" s="5">
         <v>5</v>
@@ -2316,27 +2360,24 @@
       <c r="E56" s="1">
         <v>1</v>
       </c>
-      <c r="K56" s="1">
-        <v>1</v>
-      </c>
-      <c r="O56" s="1">
+      <c r="L56" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="D57" s="5">
         <v>5</v>
       </c>
-      <c r="H57" s="1">
+      <c r="E57" s="1">
         <v>1</v>
       </c>
       <c r="L57" s="1">
@@ -2351,21 +2392,24 @@
         <v>13</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="D58" s="5">
         <v>5</v>
       </c>
-      <c r="H58" s="1">
-        <v>1</v>
-      </c>
-      <c r="L58" s="1">
-        <v>1</v>
-      </c>
-      <c r="N58" s="1">
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+      <c r="O58" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2374,61 +2418,64 @@
         <v>13</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D59" s="5">
         <v>5</v>
       </c>
-      <c r="H59" s="1">
-        <v>1</v>
-      </c>
-      <c r="L59" s="1">
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="K59" s="1">
+        <v>1</v>
+      </c>
+      <c r="O59" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D60" s="5">
         <v>5</v>
       </c>
-      <c r="G60" s="1">
-        <v>1</v>
-      </c>
-      <c r="J60" s="1">
-        <v>1</v>
-      </c>
-      <c r="N60" s="1">
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="L60" s="1">
+        <v>1</v>
+      </c>
+      <c r="O60" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D61" s="5">
         <v>5</v>
       </c>
-      <c r="G61" s="1">
-        <v>1</v>
-      </c>
-      <c r="J61" s="1">
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="L61" s="1">
         <v>1</v>
       </c>
       <c r="N61" s="1">
@@ -2437,27 +2484,21 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D62" s="5">
         <v>5</v>
       </c>
-      <c r="G62" s="1">
-        <v>1</v>
-      </c>
-      <c r="J62" s="1">
-        <v>1</v>
-      </c>
-      <c r="K62" s="1">
-        <v>1</v>
-      </c>
-      <c r="N62" s="1">
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="L62" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2466,21 +2507,18 @@
         <v>11</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D63" s="5">
         <v>5</v>
       </c>
-      <c r="E63" s="1">
+      <c r="G63" s="1">
         <v>1</v>
       </c>
       <c r="J63" s="1">
-        <v>1</v>
-      </c>
-      <c r="K63" s="1">
         <v>1</v>
       </c>
       <c r="N63" s="1">
@@ -2492,18 +2530,18 @@
         <v>11</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D64" s="5">
         <v>5</v>
       </c>
-      <c r="E64" s="1">
-        <v>1</v>
-      </c>
-      <c r="K64" s="1">
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1">
         <v>1</v>
       </c>
       <c r="N64" s="1">
@@ -2515,15 +2553,18 @@
         <v>12</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D65" s="5">
         <v>5</v>
       </c>
-      <c r="E65" s="1">
+      <c r="G65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
         <v>1</v>
       </c>
       <c r="K65" s="1">
@@ -2535,27 +2576,27 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G66" s="1">
+        <v>111</v>
+      </c>
+      <c r="D66" s="5">
+        <v>5</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1">
         <v>1</v>
       </c>
       <c r="K66" s="1">
         <v>1</v>
       </c>
-      <c r="L66" s="1">
-        <v>1</v>
-      </c>
-      <c r="O66" s="1">
+      <c r="N66" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2564,64 +2605,70 @@
         <v>11</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G67" s="1">
-        <v>1</v>
-      </c>
-      <c r="L67" s="1">
-        <v>1</v>
-      </c>
-      <c r="O67" s="1">
+        <v>103</v>
+      </c>
+      <c r="D67" s="5">
+        <v>5</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="K67" s="1">
+        <v>1</v>
+      </c>
+      <c r="N67" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G68" s="1">
+        <v>89</v>
+      </c>
+      <c r="D68" s="5">
+        <v>5</v>
+      </c>
+      <c r="E68" s="1">
         <v>1</v>
       </c>
       <c r="K68" s="1">
         <v>1</v>
       </c>
-      <c r="O68" s="1">
+      <c r="N68" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D69" s="5">
-        <v>5</v>
-      </c>
-      <c r="F69" s="1">
-        <v>1</v>
-      </c>
-      <c r="J69" s="1">
+        <v>113</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G69" s="1">
+        <v>1</v>
+      </c>
+      <c r="K69" s="1">
+        <v>1</v>
+      </c>
+      <c r="L69" s="1">
+        <v>1</v>
+      </c>
+      <c r="O69" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2630,18 +2677,21 @@
         <v>11</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D70" s="5">
-        <v>5</v>
-      </c>
-      <c r="F70" s="1">
+        <v>114</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G70" s="1">
         <v>1</v>
       </c>
       <c r="L70" s="1">
+        <v>1</v>
+      </c>
+      <c r="O70" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2650,18 +2700,21 @@
         <v>11</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D71" s="5">
-        <v>5</v>
-      </c>
-      <c r="F71" s="1">
-        <v>1</v>
-      </c>
-      <c r="L71" s="1">
+        <v>115</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G71" s="1">
+        <v>1</v>
+      </c>
+      <c r="K71" s="1">
+        <v>1</v>
+      </c>
+      <c r="O71" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2670,21 +2723,18 @@
         <v>11</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>155</v>
+        <v>117</v>
+      </c>
+      <c r="D72" s="5">
+        <v>5</v>
       </c>
       <c r="F72" s="1">
         <v>1</v>
       </c>
       <c r="J72" s="1">
-        <v>1</v>
-      </c>
-      <c r="O72" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2693,44 +2743,38 @@
         <v>11</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>155</v>
+        <v>98</v>
+      </c>
+      <c r="D73" s="5">
+        <v>5</v>
       </c>
       <c r="F73" s="1">
         <v>1</v>
       </c>
-      <c r="J73" s="1">
-        <v>1</v>
-      </c>
-      <c r="O73" s="1">
+      <c r="L73" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>155</v>
+        <v>118</v>
+      </c>
+      <c r="D74" s="5">
+        <v>5</v>
       </c>
       <c r="F74" s="1">
         <v>1</v>
       </c>
-      <c r="K74" s="1">
-        <v>1</v>
-      </c>
-      <c r="N74" s="1">
+      <c r="L74" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2739,10 +2783,10 @@
         <v>11</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>155</v>
@@ -2751,6 +2795,9 @@
         <v>1</v>
       </c>
       <c r="J75" s="1">
+        <v>1</v>
+      </c>
+      <c r="O75" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2759,10 +2806,10 @@
         <v>11</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>155</v>
@@ -2770,24 +2817,33 @@
       <c r="F76" s="1">
         <v>1</v>
       </c>
+      <c r="J76" s="1">
+        <v>1</v>
+      </c>
+      <c r="O76" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D77" s="5">
-        <v>5</v>
-      </c>
-      <c r="E77" s="1">
-        <v>1</v>
-      </c>
-      <c r="J77" s="1">
+        <v>121</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F77" s="1">
+        <v>1</v>
+      </c>
+      <c r="K77" s="1">
+        <v>1</v>
+      </c>
+      <c r="N77" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2796,15 +2852,18 @@
         <v>11</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D78" s="5">
-        <v>5</v>
-      </c>
-      <c r="E78" s="1">
+        <v>123</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F78" s="1">
+        <v>1</v>
+      </c>
+      <c r="J78" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2813,18 +2872,15 @@
         <v>11</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D79" s="5">
-        <v>5</v>
-      </c>
-      <c r="E79" s="1">
-        <v>1</v>
-      </c>
-      <c r="N79" s="1">
+        <v>63</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F79" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2833,10 +2889,10 @@
         <v>11</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D80" s="5">
         <v>5</v>
@@ -2844,7 +2900,7 @@
       <c r="E80" s="1">
         <v>1</v>
       </c>
-      <c r="O80" s="1">
+      <c r="J80" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2853,18 +2909,15 @@
         <v>11</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="D81" s="5">
         <v>5</v>
       </c>
       <c r="E81" s="1">
-        <v>1</v>
-      </c>
-      <c r="N81" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2873,18 +2926,18 @@
         <v>11</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="D82" s="5">
         <v>5</v>
       </c>
-      <c r="H82" s="1">
-        <v>1</v>
-      </c>
-      <c r="O82" s="1">
+      <c r="E82" s="1">
+        <v>1</v>
+      </c>
+      <c r="N82" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2893,18 +2946,15 @@
         <v>11</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D83" s="5">
         <v>5</v>
       </c>
-      <c r="H83" s="1">
-        <v>1</v>
-      </c>
-      <c r="K83" s="1">
+      <c r="E83" s="1">
         <v>1</v>
       </c>
       <c r="O83" s="1">
@@ -2916,42 +2966,38 @@
         <v>11</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
       <c r="D84" s="5">
         <v>5</v>
       </c>
-      <c r="H84" s="1">
-        <v>1</v>
-      </c>
-      <c r="O84" s="1">
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+      <c r="N84" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C85" s="2"/>
-      <c r="D85" s="5" t="s">
-        <v>155</v>
+        <v>29</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D85" s="5">
+        <v>5</v>
       </c>
       <c r="H85" s="1">
         <v>1</v>
       </c>
-      <c r="J85" s="1">
-        <v>1</v>
-      </c>
       <c r="L85" s="1">
-        <v>1</v>
-      </c>
-      <c r="M85" s="1">
         <v>1</v>
       </c>
       <c r="O85" s="1">
@@ -2960,13 +3006,13 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D86" s="5">
         <v>5</v>
@@ -2974,31 +3020,22 @@
       <c r="H86" s="1">
         <v>1</v>
       </c>
-      <c r="J86" s="1">
-        <v>1</v>
-      </c>
       <c r="K86" s="1">
         <v>1</v>
       </c>
-      <c r="L86" s="1">
-        <v>1</v>
-      </c>
-      <c r="M86" s="1">
-        <v>1</v>
-      </c>
-      <c r="N86" s="1">
+      <c r="O86" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D87" s="5">
         <v>5</v>
@@ -3006,7 +3043,7 @@
       <c r="H87" s="1">
         <v>1</v>
       </c>
-      <c r="M87" s="1">
+      <c r="L87" s="1">
         <v>1</v>
       </c>
       <c r="O87" s="1">
@@ -3018,25 +3055,25 @@
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C88" s="2"/>
-      <c r="D88" s="5">
-        <v>5</v>
-      </c>
-      <c r="G88" s="1">
+      <c r="D88" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H88" s="1">
         <v>1</v>
       </c>
       <c r="J88" s="1">
         <v>1</v>
       </c>
-      <c r="K88" s="1">
+      <c r="L88" s="1">
         <v>1</v>
       </c>
       <c r="M88" s="1">
         <v>1</v>
       </c>
-      <c r="N88" s="1">
+      <c r="O88" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3045,44 +3082,47 @@
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G89" s="1">
+        <v>132</v>
+      </c>
+      <c r="D89" s="5">
+        <v>5</v>
+      </c>
+      <c r="H89" s="1">
         <v>1</v>
       </c>
       <c r="J89" s="1">
         <v>1</v>
       </c>
+      <c r="K89" s="1">
+        <v>1</v>
+      </c>
+      <c r="L89" s="1">
+        <v>1</v>
+      </c>
       <c r="M89" s="1">
         <v>1</v>
       </c>
-      <c r="O89" s="1">
+      <c r="N89" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G90" s="1">
-        <v>1</v>
-      </c>
-      <c r="J90" s="1">
+        <v>133</v>
+      </c>
+      <c r="D90" s="5">
+        <v>5</v>
+      </c>
+      <c r="H90" s="1">
         <v>1</v>
       </c>
       <c r="M90" s="1">
@@ -3097,16 +3137,15 @@
         <v>8</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C91" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="D91" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G91" s="1">
-        <v>1</v>
-      </c>
-      <c r="J91" s="1">
+        <v>159</v>
+      </c>
+      <c r="H91" s="1">
         <v>1</v>
       </c>
       <c r="M91" s="1">
@@ -3121,22 +3160,25 @@
         <v>8</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" s="5">
         <v>5</v>
       </c>
-      <c r="F92" s="1">
+      <c r="G92" s="1">
+        <v>1</v>
+      </c>
+      <c r="J92" s="1">
         <v>1</v>
       </c>
       <c r="K92" s="1">
         <v>1</v>
       </c>
-      <c r="L92" s="1">
-        <v>1</v>
-      </c>
       <c r="M92" s="1">
+        <v>1</v>
+      </c>
+      <c r="N92" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3145,16 +3187,18 @@
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="5">
-        <v>5</v>
-      </c>
-      <c r="H93" s="1">
-        <v>1</v>
-      </c>
-      <c r="L93" s="1">
+        <v>135</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1</v>
+      </c>
+      <c r="J93" s="1">
         <v>1</v>
       </c>
       <c r="M93" s="1">
@@ -3169,13 +3213,18 @@
         <v>8</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="5">
-        <v>5</v>
-      </c>
-      <c r="F94" s="1">
+        <v>136</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G94" s="1">
+        <v>1</v>
+      </c>
+      <c r="J94" s="1">
         <v>1</v>
       </c>
       <c r="M94" s="1">
@@ -3190,19 +3239,16 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E95" s="1">
+      <c r="G95" s="1">
         <v>1</v>
       </c>
       <c r="J95" s="1">
-        <v>1</v>
-      </c>
-      <c r="K95" s="1">
         <v>1</v>
       </c>
       <c r="M95" s="1">
@@ -3214,37 +3260,40 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>6</v>
+        <v>139</v>
       </c>
       <c r="C96" s="2"/>
-      <c r="D96" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="G96" s="1">
+      <c r="D96" s="5">
+        <v>5</v>
+      </c>
+      <c r="F96" s="1">
+        <v>1</v>
+      </c>
+      <c r="K96" s="1">
+        <v>1</v>
+      </c>
+      <c r="L96" s="1">
         <v>1</v>
       </c>
       <c r="M96" s="1">
-        <v>1</v>
-      </c>
-      <c r="O96" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="5">
         <v>5</v>
       </c>
-      <c r="E97" s="1">
+      <c r="H97" s="1">
         <v>1</v>
       </c>
       <c r="L97" s="1">
@@ -3253,58 +3302,55 @@
       <c r="M97" s="1">
         <v>1</v>
       </c>
-      <c r="N97" s="1">
+      <c r="O97" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="5">
         <v>5</v>
       </c>
-      <c r="E98" s="1">
-        <v>1</v>
-      </c>
-      <c r="J98" s="1">
-        <v>1</v>
-      </c>
-      <c r="K98" s="1">
+      <c r="F98" s="1">
         <v>1</v>
       </c>
       <c r="M98" s="1">
         <v>1</v>
       </c>
-      <c r="N98" s="1">
+      <c r="O98" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E99" s="1">
         <v>1</v>
       </c>
-      <c r="L99" s="1">
+      <c r="J99" s="1">
+        <v>1</v>
+      </c>
+      <c r="K99" s="1">
         <v>1</v>
       </c>
       <c r="M99" s="1">
         <v>1</v>
       </c>
-      <c r="O99" s="1">
+      <c r="N99" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3313,16 +3359,13 @@
         <v>1</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>143</v>
+        <v>6</v>
       </c>
       <c r="C100" s="2"/>
-      <c r="D100" s="5">
-        <v>5</v>
-      </c>
-      <c r="E100" s="1">
-        <v>1</v>
-      </c>
-      <c r="L100" s="1">
+      <c r="D100" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G100" s="1">
         <v>1</v>
       </c>
       <c r="M100" s="1">
@@ -3337,19 +3380,15 @@
         <v>1</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C101" s="2"/>
+        <v>163</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="D101" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G101" s="1">
-        <v>1</v>
-      </c>
-      <c r="J101" s="1">
-        <v>1</v>
-      </c>
-      <c r="K101" s="1">
+        <v>157</v>
+      </c>
+      <c r="H101" s="1">
         <v>1</v>
       </c>
       <c r="M101" s="1">
@@ -3364,22 +3403,27 @@
         <v>1</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C102" s="2"/>
-      <c r="D102" s="5">
-        <v>5</v>
-      </c>
-      <c r="G102" s="1">
-        <v>1</v>
-      </c>
-      <c r="J102" s="1">
+        <v>163</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H102" s="1">
+        <v>1</v>
+      </c>
+      <c r="K102" s="1">
+        <v>1</v>
+      </c>
+      <c r="L102" s="1">
         <v>1</v>
       </c>
       <c r="M102" s="1">
         <v>1</v>
       </c>
-      <c r="N102" s="1">
+      <c r="O102" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3388,22 +3432,24 @@
         <v>1</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C103" s="2"/>
-      <c r="D103" s="5">
-        <v>5</v>
-      </c>
-      <c r="G103" s="1">
-        <v>1</v>
-      </c>
-      <c r="K103" s="1">
+        <v>163</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H103" s="1">
+        <v>1</v>
+      </c>
+      <c r="J103" s="1">
         <v>1</v>
       </c>
       <c r="M103" s="1">
         <v>1</v>
       </c>
-      <c r="O103" s="1">
+      <c r="N103" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3412,70 +3458,73 @@
         <v>1</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C104" s="2"/>
-      <c r="D104" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="I104" s="1">
-        <v>1</v>
-      </c>
-      <c r="J104" s="1">
-        <v>1</v>
-      </c>
-      <c r="K104" s="1">
+      <c r="D104" s="5">
+        <v>5</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="L104" s="1">
         <v>1</v>
       </c>
       <c r="M104" s="1">
         <v>1</v>
       </c>
-      <c r="O104" s="1">
+      <c r="N104" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="5">
         <v>5</v>
       </c>
-      <c r="F105" s="1">
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+      <c r="J105" s="1">
+        <v>1</v>
+      </c>
+      <c r="K105" s="1">
         <v>1</v>
       </c>
       <c r="M105" s="1">
         <v>1</v>
       </c>
-      <c r="O105" s="1">
+      <c r="N105" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="C106" s="2"/>
-      <c r="D106" s="5">
-        <v>5</v>
-      </c>
-      <c r="F106" s="1">
-        <v>1</v>
-      </c>
-      <c r="J106" s="1">
+      <c r="D106" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E106" s="1">
+        <v>1</v>
+      </c>
+      <c r="L106" s="1">
         <v>1</v>
       </c>
       <c r="M106" s="1">
         <v>1</v>
       </c>
-      <c r="N106" s="1">
+      <c r="O106" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3484,13 +3533,13 @@
         <v>1</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>2</v>
+        <v>143</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="5">
         <v>5</v>
       </c>
-      <c r="F107" s="1">
+      <c r="E107" s="1">
         <v>1</v>
       </c>
       <c r="L107" s="1">
@@ -3508,30 +3557,210 @@
         <v>1</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G108" s="1">
+        <v>1</v>
+      </c>
+      <c r="J108" s="1">
+        <v>1</v>
+      </c>
+      <c r="K108" s="1">
+        <v>1</v>
+      </c>
+      <c r="M108" s="1">
+        <v>1</v>
+      </c>
+      <c r="O108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="5">
+        <v>5</v>
+      </c>
+      <c r="G109" s="1">
+        <v>1</v>
+      </c>
+      <c r="J109" s="1">
+        <v>1</v>
+      </c>
+      <c r="M109" s="1">
+        <v>1</v>
+      </c>
+      <c r="N109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="5">
+        <v>5</v>
+      </c>
+      <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="K110" s="1">
+        <v>1</v>
+      </c>
+      <c r="M110" s="1">
+        <v>1</v>
+      </c>
+      <c r="O110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I111" s="1">
+        <v>1</v>
+      </c>
+      <c r="J111" s="1">
+        <v>1</v>
+      </c>
+      <c r="K111" s="1">
+        <v>1</v>
+      </c>
+      <c r="M111" s="1">
+        <v>1</v>
+      </c>
+      <c r="O111" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="5">
+        <v>5</v>
+      </c>
+      <c r="F112" s="1">
+        <v>1</v>
+      </c>
+      <c r="M112" s="1">
+        <v>1</v>
+      </c>
+      <c r="O112" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="5">
+        <v>5</v>
+      </c>
+      <c r="F113" s="1">
+        <v>1</v>
+      </c>
+      <c r="J113" s="1">
+        <v>1</v>
+      </c>
+      <c r="M113" s="1">
+        <v>1</v>
+      </c>
+      <c r="N113" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="5">
+        <v>5</v>
+      </c>
+      <c r="F114" s="1">
+        <v>1</v>
+      </c>
+      <c r="L114" s="1">
+        <v>1</v>
+      </c>
+      <c r="M114" s="1">
+        <v>1</v>
+      </c>
+      <c r="O114" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="2"/>
-      <c r="D108" s="5">
-        <v>5</v>
-      </c>
-      <c r="H108" s="1">
-        <v>1</v>
-      </c>
-      <c r="K108" s="1">
-        <v>1</v>
-      </c>
-      <c r="L108" s="1">
-        <v>1</v>
-      </c>
-      <c r="M108" s="1">
-        <v>1</v>
-      </c>
-      <c r="O108" s="1">
-        <v>1</v>
-      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="5">
+        <v>5</v>
+      </c>
+      <c r="H115" s="1">
+        <v>1</v>
+      </c>
+      <c r="K115" s="1">
+        <v>1</v>
+      </c>
+      <c r="L115" s="1">
+        <v>1</v>
+      </c>
+      <c r="M115" s="1">
+        <v>1</v>
+      </c>
+      <c r="O115" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B118" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O115" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fix: weight of 埃迪卡拉级
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -1,34 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\work\tc\lagrange\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D01A9C-34D0-473A-87A3-0ED22044D86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F99627-BD1F-460D-8118-2039B077CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1997" yWindow="3146" windowWidth="25963" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="29306" windowHeight="15909" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="保底" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">保底!$A$1:$O$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">保底!$A$1:$O$120</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="168">
   <si>
     <t>SC002</t>
   </si>
@@ -622,10 +633,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>概率</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>支援舰</t>
   </si>
   <si>
@@ -641,34 +648,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2.5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>S-列维9号</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>雷火之星</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>埃迪卡拉级</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -693,15 +680,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>高速型(C)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>雨海级</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BR050</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御型(B)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼雷型(C)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>权重</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -709,6 +708,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.000_);[Red]\(0.000\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -761,7 +764,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -779,6 +782,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,13 +1070,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O120"/>
+  <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D77" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D90" sqref="D90"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -1076,10 +1085,14 @@
     <col min="2" max="2" width="16.3828125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.3828125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.3828125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="15" width="9" style="1"/>
+    <col min="16" max="16" width="9" style="7"/>
+    <col min="17" max="17" width="9.3046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="6"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1090,7 +1103,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>33</v>
@@ -1105,7 +1118,7 @@
         <v>34</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>35</v>
@@ -1126,7 +1139,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1149,8 +1162,11 @@
       <c r="O2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1167,8 +1183,11 @@
       <c r="L3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1185,17 +1204,18 @@
       <c r="L4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="5" t="s">
-        <v>161</v>
+      <c r="D5" s="2">
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -1209,8 +1229,11 @@
       <c r="O5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1234,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1254,8 +1277,11 @@
       <c r="O7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1263,8 +1289,8 @@
         <v>43</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="5" t="s">
-        <v>155</v>
+      <c r="D8" s="2">
+        <v>2.5</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -1278,8 +1304,10 @@
       <c r="O8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1299,38 +1327,42 @@
       <c r="O9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1</v>
-      </c>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="5" t="s">
-        <v>155</v>
+      <c r="D11" s="2">
+        <v>2.5</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1341,8 +1373,10 @@
       <c r="L11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1364,8 +1398,11 @@
       <c r="O12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1387,8 +1424,11 @@
       <c r="O13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1407,8 +1447,11 @@
       <c r="L14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1430,8 +1473,11 @@
       <c r="O15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1450,8 +1496,11 @@
       <c r="L16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1470,8 +1519,11 @@
       <c r="L17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1490,8 +1542,11 @@
       <c r="L18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -1543,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1566,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -1585,8 +1640,9 @@
       <c r="N22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -1608,8 +1664,9 @@
       <c r="N23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1631,8 +1688,9 @@
       <c r="N24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1654,8 +1712,11 @@
       <c r="N25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="1"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1677,8 +1738,11 @@
       <c r="N26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="1"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1697,8 +1761,11 @@
       <c r="N27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
@@ -1723,8 +1790,10 @@
       <c r="O28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="4"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -1749,8 +1818,10 @@
       <c r="O29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="1"/>
+      <c r="Q29" s="4"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
@@ -1775,8 +1846,10 @@
       <c r="O30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1801,8 +1874,10 @@
       <c r="N31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
@@ -1824,8 +1899,11 @@
       <c r="O32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -1841,8 +1919,11 @@
       <c r="H33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -1850,10 +1931,10 @@
         <v>71</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="D34" s="5">
+        <v>5</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
@@ -1861,8 +1942,11 @@
       <c r="L34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1887,8 +1971,11 @@
       <c r="N35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1910,8 +1997,11 @@
       <c r="O36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
@@ -1930,8 +2020,11 @@
       <c r="O37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -1947,8 +2040,11 @@
       <c r="H38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -1974,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2000,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -2022,8 +2118,11 @@
       <c r="O41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="1"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
@@ -2045,8 +2144,11 @@
       <c r="N42" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="1"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>13</v>
       </c>
@@ -2065,8 +2167,11 @@
       <c r="N43" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -2088,8 +2193,11 @@
       <c r="N44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>13</v>
       </c>
@@ -2114,8 +2222,10 @@
       <c r="O45" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="1"/>
+      <c r="Q45" s="4"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
@@ -2137,8 +2247,11 @@
       <c r="N46" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46" s="1"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
@@ -2160,8 +2273,11 @@
       <c r="N47" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47" s="1"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -2186,8 +2302,10 @@
       <c r="N48" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48" s="1"/>
+      <c r="Q48" s="7"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
@@ -2206,8 +2324,9 @@
       <c r="L49" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>14</v>
       </c>
@@ -2226,8 +2345,9 @@
       <c r="L50" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R50" s="1"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>13</v>
       </c>
@@ -2253,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
@@ -2279,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -2305,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>13</v>
       </c>
@@ -2324,8 +2444,11 @@
       <c r="L54" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
@@ -2344,8 +2467,11 @@
       <c r="L55" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
@@ -2364,8 +2490,11 @@
       <c r="L56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>13</v>
       </c>
@@ -2387,8 +2516,11 @@
       <c r="O57" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>13</v>
       </c>
@@ -2413,8 +2545,10 @@
       <c r="O58" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58" s="1"/>
+      <c r="Q58" s="4"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>13</v>
       </c>
@@ -2436,8 +2570,10 @@
       <c r="O59" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59" s="1"/>
+      <c r="Q59" s="7"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>14</v>
       </c>
@@ -2459,8 +2595,11 @@
       <c r="O60" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>13</v>
       </c>
@@ -2482,8 +2621,11 @@
       <c r="N61" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>13</v>
       </c>
@@ -2502,8 +2644,11 @@
       <c r="L62" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -2525,8 +2670,11 @@
       <c r="N63" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63" s="1"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
@@ -2548,8 +2696,11 @@
       <c r="N64" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64" s="1"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>12</v>
       </c>
@@ -2574,8 +2725,10 @@
       <c r="N65" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65" s="1"/>
+      <c r="Q65" s="4"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
@@ -2600,8 +2753,10 @@
       <c r="N66" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66" s="1"/>
+      <c r="Q66" s="4"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
@@ -2623,8 +2778,10 @@
       <c r="N67" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P67" s="1"/>
+      <c r="Q67" s="7"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
@@ -2646,8 +2803,10 @@
       <c r="N68" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" s="1"/>
+      <c r="Q68" s="7"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>12</v>
       </c>
@@ -2657,8 +2816,8 @@
       <c r="C69" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>157</v>
+      <c r="D69" s="5">
+        <v>5</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
@@ -2672,8 +2831,10 @@
       <c r="O69" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69" s="1"/>
+      <c r="Q69" s="7"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
@@ -2683,8 +2844,8 @@
       <c r="C70" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>157</v>
+      <c r="D70" s="5">
+        <v>5</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -2695,8 +2856,11 @@
       <c r="O70" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -2706,8 +2870,8 @@
       <c r="C71" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>155</v>
+      <c r="D71" s="2">
+        <v>2.5</v>
       </c>
       <c r="G71" s="1">
         <v>1</v>
@@ -2718,8 +2882,10 @@
       <c r="O71" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71" s="1"/>
+      <c r="Q71" s="7"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
@@ -2738,8 +2904,9 @@
       <c r="J72" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R72" s="4"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>11</v>
       </c>
@@ -2758,8 +2925,9 @@
       <c r="L73" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R73" s="1"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>11</v>
       </c>
@@ -2778,8 +2946,9 @@
       <c r="L74" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R74" s="1"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -2789,8 +2958,8 @@
       <c r="C75" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>155</v>
+      <c r="D75" s="2">
+        <v>2.5</v>
       </c>
       <c r="F75" s="1">
         <v>1</v>
@@ -2801,8 +2970,9 @@
       <c r="O75" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R75" s="4"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
@@ -2812,8 +2982,8 @@
       <c r="C76" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>155</v>
+      <c r="D76" s="2">
+        <v>2.5</v>
       </c>
       <c r="F76" s="1">
         <v>1</v>
@@ -2824,8 +2994,9 @@
       <c r="O76" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R76" s="4"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>12</v>
       </c>
@@ -2835,8 +3006,8 @@
       <c r="C77" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="5" t="s">
-        <v>155</v>
+      <c r="D77" s="2">
+        <v>2.5</v>
       </c>
       <c r="F77" s="1">
         <v>1</v>
@@ -2848,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
@@ -2858,8 +3029,8 @@
       <c r="C78" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>155</v>
+      <c r="D78" s="2">
+        <v>2.5</v>
       </c>
       <c r="F78" s="1">
         <v>1</v>
@@ -2867,8 +3038,9 @@
       <c r="J78" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R78" s="4"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
@@ -2878,14 +3050,15 @@
       <c r="C79" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>155</v>
+      <c r="D79" s="2">
+        <v>2.5</v>
       </c>
       <c r="F79" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R79" s="1"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>11</v>
       </c>
@@ -2904,8 +3077,11 @@
       <c r="J80" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80" s="1"/>
+      <c r="Q80" s="4"/>
+      <c r="R80" s="4"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
@@ -2921,8 +3097,11 @@
       <c r="E81" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
@@ -2941,8 +3120,11 @@
       <c r="N82" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -2961,8 +3143,11 @@
       <c r="O83" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
@@ -2981,8 +3166,11 @@
       <c r="N84" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
@@ -3004,8 +3192,11 @@
       <c r="O85" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>11</v>
       </c>
@@ -3027,8 +3218,10 @@
       <c r="O86" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P86" s="1"/>
+      <c r="Q86" s="7"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>11</v>
       </c>
@@ -3050,19 +3243,22 @@
       <c r="O87" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D88" s="5" t="s">
-        <v>155</v>
+      <c r="D88" s="2">
+        <v>2.5</v>
       </c>
       <c r="E88" s="1">
         <v>1</v>
@@ -3073,19 +3269,22 @@
       <c r="O88" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88" s="1"/>
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D89" s="5" t="s">
-        <v>155</v>
+      <c r="D89" s="2">
+        <v>2.5</v>
       </c>
       <c r="E89" s="1">
         <v>1</v>
@@ -3096,8 +3295,11 @@
       <c r="O89" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89" s="1"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -3105,8 +3307,8 @@
         <v>134</v>
       </c>
       <c r="C90" s="2"/>
-      <c r="D90" s="5" t="s">
-        <v>155</v>
+      <c r="D90" s="2">
+        <v>2.5</v>
       </c>
       <c r="H90" s="1">
         <v>1</v>
@@ -3123,8 +3325,11 @@
       <c r="O90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P90" s="4"/>
+      <c r="Q90" s="4"/>
+      <c r="R90" s="4"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -3155,8 +3360,10 @@
       <c r="N91" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>10</v>
       </c>
@@ -3178,8 +3385,11 @@
       <c r="O92" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -3187,10 +3397,10 @@
         <v>30</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>159</v>
+        <v>162</v>
+      </c>
+      <c r="D93" s="2">
+        <v>5</v>
       </c>
       <c r="H93" s="1">
         <v>1</v>
@@ -3201,8 +3411,11 @@
       <c r="N93" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>8</v>
       </c>
@@ -3228,8 +3441,10 @@
       <c r="N94" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94" s="1"/>
+      <c r="Q94" s="4"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>8</v>
       </c>
@@ -3239,8 +3454,8 @@
       <c r="C95" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D95" s="5" t="s">
-        <v>157</v>
+      <c r="D95" s="2">
+        <v>5</v>
       </c>
       <c r="G95" s="1">
         <v>1</v>
@@ -3254,8 +3469,11 @@
       <c r="O95" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P95" s="1"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>8</v>
       </c>
@@ -3265,8 +3483,8 @@
       <c r="C96" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D96" s="5" t="s">
-        <v>155</v>
+      <c r="D96" s="2">
+        <v>2.5</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
@@ -3280,8 +3498,11 @@
       <c r="O96" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96" s="1"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
@@ -3289,8 +3510,8 @@
         <v>138</v>
       </c>
       <c r="C97" s="2"/>
-      <c r="D97" s="5" t="s">
-        <v>155</v>
+      <c r="D97" s="2">
+        <v>2.5</v>
       </c>
       <c r="G97" s="1">
         <v>1</v>
@@ -3304,8 +3525,11 @@
       <c r="N97" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P97" s="1"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>8</v>
       </c>
@@ -3332,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>8</v>
       </c>
@@ -3355,8 +3579,11 @@
       <c r="O99" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="1"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
@@ -3376,17 +3603,18 @@
       <c r="O100" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R100" s="1"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C101" s="2"/>
-      <c r="D101" s="5" t="s">
-        <v>155</v>
+      <c r="D101" s="2">
+        <v>2.5</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -3403,8 +3631,10 @@
       <c r="N101" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P101" s="1"/>
+      <c r="Q101" s="4"/>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>1</v>
       </c>
@@ -3412,8 +3642,8 @@
         <v>6</v>
       </c>
       <c r="C102" s="2"/>
-      <c r="D102" s="5" t="s">
-        <v>155</v>
+      <c r="D102" s="2">
+        <v>2.5</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
@@ -3424,71 +3654,79 @@
       <c r="O102" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+      <c r="R102" s="1"/>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D103" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D103" s="2">
+        <v>5</v>
+      </c>
+      <c r="H103" s="1">
+        <v>1</v>
+      </c>
+      <c r="M103" s="1">
+        <v>1</v>
+      </c>
+      <c r="O103" s="1">
+        <v>1</v>
+      </c>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+      <c r="R103" s="1"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H103" s="1">
-        <v>1</v>
-      </c>
-      <c r="M103" s="1">
-        <v>1</v>
-      </c>
-      <c r="O103" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C104" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D104" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D104" s="2">
+        <v>5</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1</v>
+      </c>
+      <c r="K104" s="1">
+        <v>1</v>
+      </c>
+      <c r="L104" s="1">
+        <v>1</v>
+      </c>
+      <c r="M104" s="1">
+        <v>1</v>
+      </c>
+      <c r="O104" s="1">
+        <v>1</v>
+      </c>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="7"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H104" s="1">
-        <v>1</v>
-      </c>
-      <c r="K104" s="1">
-        <v>1</v>
-      </c>
-      <c r="L104" s="1">
-        <v>1</v>
-      </c>
-      <c r="M104" s="1">
-        <v>1</v>
-      </c>
-      <c r="O104" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="C105" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
+      </c>
+      <c r="D105" s="2">
+        <v>2.5</v>
       </c>
       <c r="H105" s="1">
         <v>1</v>
@@ -3502,8 +3740,11 @@
       <c r="N105" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P105" s="4"/>
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>1</v>
       </c>
@@ -3526,8 +3767,11 @@
       <c r="N106" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+      <c r="R106" s="1"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -3553,8 +3797,10 @@
       <c r="N107" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P107" s="1"/>
+      <c r="Q107" s="4"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>4</v>
       </c>
@@ -3562,8 +3808,8 @@
         <v>142</v>
       </c>
       <c r="C108" s="2"/>
-      <c r="D108" s="5" t="s">
-        <v>158</v>
+      <c r="D108" s="2">
+        <v>2.5</v>
       </c>
       <c r="E108" s="1">
         <v>1</v>
@@ -3577,8 +3823,11 @@
       <c r="O108" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+      <c r="R108" s="1"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>1</v>
       </c>
@@ -3601,8 +3850,11 @@
       <c r="O109" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+      <c r="R109" s="1"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>1</v>
       </c>
@@ -3610,8 +3862,8 @@
         <v>144</v>
       </c>
       <c r="C110" s="2"/>
-      <c r="D110" s="5" t="s">
-        <v>158</v>
+      <c r="D110" s="2">
+        <v>2.5</v>
       </c>
       <c r="G110" s="1">
         <v>1</v>
@@ -3628,8 +3880,10 @@
       <c r="O110" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P110" s="1"/>
+      <c r="Q110" s="4"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>1</v>
       </c>
@@ -3652,8 +3906,11 @@
       <c r="N111" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P111" s="1"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>1</v>
       </c>
@@ -3676,17 +3933,19 @@
       <c r="O112" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P112" s="1"/>
+      <c r="Q112" s="7"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C113" s="2"/>
-      <c r="D113" s="5" t="s">
-        <v>158</v>
+      <c r="D113" s="2">
+        <v>2.5</v>
       </c>
       <c r="I113" s="1">
         <v>1</v>
@@ -3703,8 +3962,10 @@
       <c r="O113" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P113" s="1"/>
+      <c r="Q113" s="4"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>1</v>
       </c>
@@ -3724,8 +3985,9 @@
       <c r="O114" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R114" s="1"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>1</v>
       </c>
@@ -3748,8 +4010,9 @@
       <c r="N115" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R115" s="4"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>1</v>
       </c>
@@ -3772,8 +4035,9 @@
       <c r="O116" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R116" s="1"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
@@ -3799,18 +4063,107 @@
       <c r="O117" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B118" s="2"/>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B119" s="2"/>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B120" s="2"/>
+      <c r="P117" s="1"/>
+      <c r="Q117" s="7"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D118" s="2">
+        <v>3.76</v>
+      </c>
+      <c r="H118" s="1">
+        <v>1</v>
+      </c>
+      <c r="J118" s="1">
+        <v>1</v>
+      </c>
+      <c r="M118" s="1">
+        <v>1</v>
+      </c>
+      <c r="N118" s="1">
+        <v>1</v>
+      </c>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D119" s="2">
+        <v>5</v>
+      </c>
+      <c r="H119" s="1">
+        <v>1</v>
+      </c>
+      <c r="K119" s="1">
+        <v>1</v>
+      </c>
+      <c r="M119" s="1">
+        <v>1</v>
+      </c>
+      <c r="N119" s="1">
+        <v>1</v>
+      </c>
+      <c r="P119" s="1"/>
+      <c r="Q119" s="7"/>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D120" s="2">
+        <v>3.76</v>
+      </c>
+      <c r="H120" s="1">
+        <v>1</v>
+      </c>
+      <c r="J120" s="1">
+        <v>1</v>
+      </c>
+      <c r="M120" s="1">
+        <v>1</v>
+      </c>
+      <c r="N120" s="1">
+        <v>1</v>
+      </c>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="4"/>
+      <c r="R120" s="4"/>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C121" s="2"/>
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C122" s="2"/>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C128" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O117" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O120" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>